<commit_message>
cambio por tema de cifras
</commit_message>
<xml_diff>
--- a/Resultado/informe_diario_20250408.xlsx
+++ b/Resultado/informe_diario_20250408.xlsx
@@ -88,19 +88,19 @@
     <t>Valor transacciones</t>
   </si>
   <si>
-    <t>0.44%</t>
+    <t>0.48%</t>
   </si>
   <si>
     <t>25.70%</t>
   </si>
   <si>
-    <t>22.44%</t>
-  </si>
-  <si>
-    <t>26.27%</t>
-  </si>
-  <si>
-    <t>10.14%</t>
+    <t>22.42%</t>
+  </si>
+  <si>
+    <t>26.73%</t>
+  </si>
+  <si>
+    <t>9.68%</t>
   </si>
   <si>
     <t>4.70</t>
@@ -112,13 +112,13 @@
     <t>3,660,909,639,546</t>
   </si>
   <si>
-    <t>0.30%</t>
+    <t>0.33%</t>
   </si>
   <si>
     <t>30.04%</t>
   </si>
   <si>
-    <t>21.79%</t>
+    <t>21.81%</t>
   </si>
   <si>
     <t>50.23%</t>
@@ -130,19 +130,19 @@
     <t>4,157,127,708,445</t>
   </si>
   <si>
-    <t>0.74%</t>
-  </si>
-  <si>
-    <t>55.74%</t>
-  </si>
-  <si>
-    <t>44.26%</t>
-  </si>
-  <si>
-    <t>76.5%</t>
-  </si>
-  <si>
-    <t>23.5%</t>
+    <t>0.81%</t>
+  </si>
+  <si>
+    <t>55.76%</t>
+  </si>
+  <si>
+    <t>44.24%</t>
+  </si>
+  <si>
+    <t>76.96%</t>
+  </si>
+  <si>
+    <t>23.04%</t>
   </si>
   <si>
     <t>7,818,037,347,991</t>
@@ -534,7 +534,7 @@
         <v>8709</v>
       </c>
       <c r="D2">
-        <v>17005</v>
+        <v>16996</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -682,13 +682,13 @@
         <v>15</v>
       </c>
       <c r="B13">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C13">
         <v>109</v>
       </c>
       <c r="D13">
-        <v>166</v>
+        <v>167</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -696,13 +696,13 @@
         <v>16</v>
       </c>
       <c r="B14">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C14">
         <v>29</v>
       </c>
       <c r="D14">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="15" spans="1:4">

</xml_diff>